<commit_message>
updated Kapazitätenplan & Projektstrukturplan
</commit_message>
<xml_diff>
--- a/doc/ProjectOrder/4.1Projektstrukturplan.xlsx
+++ b/doc/ProjectOrder/4.1Projektstrukturplan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="15133" yWindow="0" windowWidth="18419" windowHeight="15487" tabRatio="309"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$R$13</definedName>
     <definedName name="Print_Area_0" localSheetId="0">Tabelle1!$A$1:$R$13</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
-  <si>
-    <t>ASTTN-Framework</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Projektvorbereitung</t>
   </si>
@@ -137,13 +134,22 @@
   </si>
   <si>
     <t>4.1 Projektstrukturplan</t>
+  </si>
+  <si>
+    <t>Testgebiet erkunden</t>
+  </si>
+  <si>
+    <t>Klare Sicht im Kupfergraben</t>
+  </si>
+  <si>
+    <t>Testorte erkunden und festlegen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -252,11 +258,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -281,8 +284,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -368,7 +380,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -442,7 +454,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -477,7 +488,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -653,426 +663,438 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="2.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.25" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.25" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.25" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.25" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.25" style="2" customWidth="1"/>
-    <col min="13" max="13" width="20.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="2.875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.25" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" style="2" customWidth="1"/>
-    <col min="17" max="17" width="2.875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="6.25" style="2" customWidth="1"/>
-    <col min="19" max="1025" width="18.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.21875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="2.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="2.88671875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.21875" style="1" customWidth="1"/>
+    <col min="19" max="1025" width="18.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="54.85" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" ht="19.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-    </row>
-    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-    </row>
-    <row r="3" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
+      <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="3">
         <v>3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="3">
         <v>4</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4"/>
+      <c r="M3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="3">
         <v>5</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4"/>
+      <c r="P3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="3">
         <v>6</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="19.5" customHeight="1">
+      <c r="H4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="5"/>
-    </row>
-    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H4"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="K5" s="3">
+        <v>40</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="3">
+        <v>50</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>60</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="19.5" customHeight="1">
+      <c r="P6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="3">
+        <v>41</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="3">
+        <v>51</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>61</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="19.5" customHeight="1">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="3">
+        <v>32</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="K9" s="3">
+        <v>42</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="3">
+        <v>52</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>62</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="19.5" customHeight="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="3">
+        <v>33</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="3">
+        <v>43</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="4">
-        <v>40</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="7" t="s">
+      <c r="M11" s="7"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" ht="19.5" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="D13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="3">
+        <v>34</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="3">
+        <v>44</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="4">
-        <v>50</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>60</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="4">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4">
-        <v>31</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4">
-        <v>41</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="4">
-        <v>51</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>61</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="4">
-        <v>32</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="4">
-        <v>42</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>62</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="D11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="4">
-        <v>23</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="4">
-        <v>33</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" s="4">
-        <v>43</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="G13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="4">
-        <v>34</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="4">
-        <v>44</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="5"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="19.5" customHeight="1">
+      <c r="H14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="22.6" customHeight="1"/>
+    <row r="17" spans="1:18" ht="61.55" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1085,14 +1107,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1025" width="10.875" customWidth="1"/>
+    <col min="1" max="1025" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1101,14 +1123,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1025" width="10.875" customWidth="1"/>
+    <col min="1" max="1025" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
small fix in Projektstrukturplan
</commit_message>
<xml_diff>
--- a/doc/ProjectOrder/4.1Projektstrukturplan.xlsx
+++ b/doc/ProjectOrder/4.1Projektstrukturplan.xlsx
@@ -63,9 +63,6 @@
     <t>4x36h</t>
   </si>
   <si>
-    <t>Stationen an Testorten betreiben</t>
-  </si>
-  <si>
     <t>6h</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Testorte erkunden und festlegen</t>
+  </si>
+  <si>
+    <t>Station(en) an Testorten betreiben</t>
   </si>
 </sst>
 </file>
@@ -284,17 +284,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -667,7 +667,7 @@
   <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -694,18 +694,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="54.85" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="G1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
       <c r="K1" s="3"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -813,23 +813,23 @@
       <c r="L5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>38</v>
+      <c r="M5" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="N5" s="3">
         <v>50</v>
       </c>
       <c r="O5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="Q5" s="3">
         <v>60</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="19.5" customHeight="1">
@@ -838,7 +838,7 @@
     </row>
     <row r="7" spans="1:18" ht="61.55" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>11</v>
@@ -847,7 +847,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3">
         <v>21</v>
@@ -856,40 +856,40 @@
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="3">
         <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="K7" s="3">
         <v>41</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="N7" s="3">
         <v>51</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q7" s="3">
         <v>61</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="19.5" customHeight="1">
@@ -900,7 +900,7 @@
     </row>
     <row r="9" spans="1:18" ht="61.55" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>12</v>
@@ -909,49 +909,49 @@
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3">
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="3">
         <v>32</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" s="3">
         <v>42</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" s="3">
         <v>52</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q9" s="3">
         <v>62</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="19.5" customHeight="1">
@@ -971,32 +971,32 @@
     <row r="11" spans="1:18" ht="61.55" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
-      <c r="D11" s="11" t="s">
-        <v>36</v>
+      <c r="D11" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="E11" s="3">
         <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="3">
         <v>33</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K11" s="3">
         <v>43</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="8"/>
@@ -1024,31 +1024,31 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="D13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="3">
         <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="3">
         <v>34</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="3">
         <v>44</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="8"/>

</xml_diff>

<commit_message>
broke up 'programing' into programig for Server and Programming of the Arduino
</commit_message>
<xml_diff>
--- a/doc/ProjectOrder/4.1Projektstrukturplan.xlsx
+++ b/doc/ProjectOrder/4.1Projektstrukturplan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Projektvorbereitung</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>SOLL-Prozess definieren</t>
-  </si>
-  <si>
-    <t>Programmierung</t>
-  </si>
-  <si>
-    <t>4x36h</t>
   </si>
   <si>
     <t>6h</t>
@@ -143,6 +137,15 @@
   </si>
   <si>
     <t>Station(en) an Testorten betreiben</t>
+  </si>
+  <si>
+    <t>4x18h</t>
+  </si>
+  <si>
+    <t>Programmierung Arduino &amp; Sensoren</t>
+  </si>
+  <si>
+    <t>Programmierung Serverseitig</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -695,13 +698,13 @@
   <sheetData>
     <row r="1" spans="1:18" ht="54.85" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="F1" s="2"/>
       <c r="G1" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -804,32 +807,32 @@
       <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>10</v>
+      <c r="J5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="K5" s="3">
         <v>40</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N5" s="3">
         <v>50</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="3">
         <v>60</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="19.5" customHeight="1">
@@ -838,7 +841,7 @@
     </row>
     <row r="7" spans="1:18" ht="61.55" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>11</v>
@@ -847,7 +850,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3">
         <v>21</v>
@@ -856,51 +859,49 @@
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3">
         <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="K7" s="3">
         <v>41</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N7" s="3">
         <v>51</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="3">
         <v>61</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="19.5" customHeight="1">
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:18" ht="61.55" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3">
         <v>12</v>
@@ -909,49 +910,49 @@
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3">
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" s="3">
         <v>32</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K9" s="3">
         <v>42</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N9" s="3">
         <v>52</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="3">
         <v>62</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="19.5" customHeight="1">
@@ -962,7 +963,6 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -972,31 +972,31 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="D11" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H11" s="3">
         <v>33</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="K11" s="3">
         <v>43</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="8"/>
@@ -1016,7 +1016,6 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
@@ -1024,31 +1023,31 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="D13" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3">
         <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H13" s="3">
         <v>34</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="K13" s="3">
         <v>44</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="8"/>
@@ -1059,7 +1058,8 @@
     </row>
     <row r="14" spans="1:18" ht="19.5" customHeight="1">
       <c r="H14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:18" ht="61.55" customHeight="1">
       <c r="A15" s="7"/>
@@ -1068,9 +1068,15 @@
       <c r="E15" s="8"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="4"/>
+      <c r="J15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="3">
+        <v>45</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="M15" s="7"/>
       <c r="N15" s="8"/>
       <c r="O15" s="4"/>

</xml_diff>